<commit_message>
Fix dopo primo deploy e gestione date creazione/modifica su Progetti, Persone e Cost Rate
</commit_message>
<xml_diff>
--- a/m_gestione/Caricatori/template/progetti-template.xlsx
+++ b/m_gestione/Caricatori/template/progetti-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aeonvisspa-my.sharepoint.com/personal/enrico_taverna_aeonvis_com/Documents/02 Development/timereport/m_gestione/Caricatori/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{71916124-2BC9-4A5F-9949-ACFD324EEB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3370646-326C-4184-8A38-00C2C06E590C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D5B75-6F07-46D9-A9F5-EB36E8475108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="403" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export opportunità per TR" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>T&amp;M</t>
   </si>
@@ -115,13 +115,16 @@
     <t>Progetto di Test 3</t>
   </si>
   <si>
-    <t>THE_888_00</t>
-  </si>
-  <si>
-    <t>FIA_888_00</t>
-  </si>
-  <si>
-    <t>THE_888_01</t>
+    <t>THE_888_02</t>
+  </si>
+  <si>
+    <t>THE_888_03</t>
+  </si>
+  <si>
+    <t>THE_888_04</t>
+  </si>
+  <si>
+    <t>ActivityOn</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,9 +551,10 @@
     <col min="11" max="11" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -593,8 +597,11 @@
       <c r="N1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -638,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -679,8 +686,11 @@
         <v>45107</v>
       </c>
       <c r="N3" s="1"/>
+      <c r="O3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
update caricatori + bug fix input ore/spese
- gestione della copia forzatura consulenti su caricatore progetti
- bug fix per evitare cancellazione della drop down list WBS alla modifica delle ore
</commit_message>
<xml_diff>
--- a/m_gestione/Caricatori/template/progetti-template.xlsx
+++ b/m_gestione/Caricatori/template/progetti-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aeonvisspa-my.sharepoint.com/personal/enrico_taverna_aeonvis_com/Documents/02 Development/timereport/m_gestione/Caricatori/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D5B75-6F07-46D9-A9F5-EB36E8475108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{4F6D5B75-6F07-46D9-A9F5-EB36E8475108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4635C749-910B-4A0A-8B20-0EEDE973FB2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="403" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>T&amp;M</t>
   </si>
@@ -125,6 +125,24 @@
   </si>
   <si>
     <t>ActivityOn</t>
+  </si>
+  <si>
+    <t>CopiaConsulentiDa</t>
+  </si>
+  <si>
+    <t>CIR_006_00</t>
+  </si>
+  <si>
+    <t>LOB</t>
+  </si>
+  <si>
+    <t>ERP</t>
+  </si>
+  <si>
+    <t>CDG</t>
+  </si>
+  <si>
+    <t>SCP</t>
   </si>
 </sst>
 </file>
@@ -218,7 +236,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -234,9 +252,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -274,7 +292,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -380,7 +398,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -522,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -530,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,18 +561,20 @@
     <col min="3" max="3" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -571,37 +591,43 @@
         <v>11</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
@@ -617,35 +643,39 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="1">
         <v>1000</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>23.2</v>
       </c>
-      <c r="L2" s="2">
+      <c r="N2" s="2">
         <v>44927</v>
       </c>
-      <c r="M2" s="2">
+      <c r="O2" s="2">
         <v>45015</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>32</v>
       </c>
@@ -661,36 +691,40 @@
       <c r="E3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="1">
+      <c r="L3" s="1">
         <v>1040</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>30.4</v>
       </c>
-      <c r="L3" s="2">
+      <c r="N3" s="2">
         <v>44972</v>
       </c>
-      <c r="M3" s="2">
+      <c r="O3" s="2">
         <v>45107</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" t="s">
+      <c r="P3" s="1"/>
+      <c r="Q3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
@@ -707,30 +741,36 @@
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="1">
+      <c r="L4" s="1">
         <v>1080</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>37.6</v>
       </c>
-      <c r="L4" s="2">
+      <c r="N4" s="2">
         <v>45017</v>
       </c>
-      <c r="M4" s="2">
+      <c r="O4" s="2">
         <v>45199</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>